<commit_message>
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C768910
</commit_message>
<xml_diff>
--- a/PPIUK-Login/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Login/src/test/resources/CobaltUsers.xlsx
@@ -1054,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="G84" sqref="A81:G84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,18 +2577,6 @@
       <c r="G80" s="10" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="9"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="9"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E83" s="9"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E84" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Update password for LoginUser3
git-tfs-id: [http://tfsnpt.int.thomson.com:8080/tfs/Cobalt_Collection]$/Cobalt QED Testing/PLPLusUK;C775594
</commit_message>
<xml_diff>
--- a/PPIUK-Login/src/test/resources/CobaltUsers.xlsx
+++ b/PPIUK-Login/src/test/resources/CobaltUsers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="274">
   <si>
     <t>UserName</t>
   </si>
@@ -844,7 +844,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1266,12 +1267,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="39.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="40.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="39.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="40.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -3437,8 +3438,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3477,13 +3478,7 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>